<commit_message>
fix(renderer): Correct missing arguments in render calls
Fixes a critical crash in the visual simulation mode and restores full rendering functionality.

The main bug was a TypeError in `renderizar_tareas_pendientes` caused by calling it with missing arguments. The fix provides the correct list of pending work orders from the dispatcher.

During the fix, a similar latent bug was identified and corrected in `renderizar_agentes`, which was also being called incorrectly.

Both fixes have been verified with a TPRF, confirming that the visual mode is now fully operational without regressions.

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/layouts/Warehouse_Logic.xlsx
+++ b/layouts/Warehouse_Logic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferri\OneDrive\Escritorio\Gemelos Digital\layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D422564-2AD6-45CF-ADB2-02681E60582D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D35160-BFEC-48E6-B56B-4BA68633AFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -584,7 +584,7 @@
   <dimension ref="A1:H361"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>